<commit_message>
Rerun NPCC contingency analysis
</commit_message>
<xml_diff>
--- a/src/notes/lmp/data/npcc_uced_base.xlsx
+++ b/src/notes/lmp/data/npcc_uced_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/psal/src/notes/lmp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFD74EE-6F3E-1647-9A46-E14A8EC5319B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4799AB13-57DC-DB4B-8062-96E40E43C4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-11540" windowWidth="21600" windowHeight="18940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="-11540" windowWidth="21600" windowHeight="18940" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="8" r:id="rId1"/>
@@ -17973,9 +17973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41866,9 +41866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41937,7 +41937,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>214</v>
+        <v>3214</v>
       </c>
       <c r="K2">
         <v>5669013.4199999999</v>
@@ -42147,7 +42147,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1826.89608</v>
+        <v>3826.89608</v>
       </c>
       <c r="K8">
         <v>172679.08900000001</v>
@@ -42287,7 +42287,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K12">
         <v>497459.73200000002</v>
@@ -42322,7 +42322,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K13">
         <v>24260.274000000001</v>
@@ -42462,7 +42462,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -42497,7 +42497,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -42532,7 +42532,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -42567,7 +42567,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K20">
         <v>837883.56200000003</v>
@@ -42602,7 +42602,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K21">
         <v>33191.7808</v>
@@ -42987,7 +42987,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -43022,7 +43022,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -43057,7 +43057,7 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -43092,7 +43092,7 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -43127,7 +43127,7 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K36">
         <v>286054.68</v>
@@ -43162,7 +43162,7 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K37">
         <v>0</v>

</xml_diff>